<commit_message>
Update data/exampleStochastic to newest formats
</commit_message>
<xml_diff>
--- a/data/exampleStochastic/Data_Packages.xlsx
+++ b/data/exampleStochastic/Data_Packages.xlsx
@@ -28,7 +28,7 @@
     <font>
       <name val="Aptos"/>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="18"/>
     </font>
     <font>
@@ -43,7 +43,7 @@
     </font>
     <font>
       <name val="Aptos"/>
-      <color rgb="000000FF"/>
+      <color rgb="FF0000FF"/>
       <sz val="11"/>
     </font>
     <font>
@@ -60,32 +60,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00008080"/>
-        <bgColor rgb="00008080"/>
+        <fgColor rgb="FF008080"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DAEEF3"/>
-        <bgColor rgb="00DAEEF3"/>
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor rgb="FFDAEEF3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D9D9D9"/>
-        <bgColor rgb="00D9D9D9"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F2F2F2"/>
-        <bgColor rgb="00F2F2F2"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFCC"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -521,7 +521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -538,9 +538,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="5.5709375" customWidth="1" min="1" max="1"/>
+    <col width="5.5703125" customWidth="1" min="1" max="1"/>
     <col width="19.7109375" customWidth="1" min="2" max="2"/>
-    <col width="24.5709375" customWidth="1" min="3" max="3"/>
+    <col width="24.5703125" customWidth="1" min="3" max="3"/>
     <col width="100.7109375" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -668,6 +668,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>